<commit_message>
Json, doc and website updates
</commit_message>
<xml_diff>
--- a/Appendix/Sprint Backlogs/SprintBacklog2nd.xlsx
+++ b/Appendix/Sprint Backlogs/SprintBacklog2nd.xlsx
@@ -983,7 +983,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,6 +1189,9 @@
       <c r="H8">
         <v>1</v>
       </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1291,6 +1294,9 @@
       <c r="H13">
         <v>4</v>
       </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1314,6 +1320,9 @@
       <c r="H14">
         <v>5</v>
       </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1337,6 +1346,9 @@
       <c r="H15">
         <v>2</v>
       </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1360,6 +1372,9 @@
       <c r="H16">
         <v>4</v>
       </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1500,6 +1515,9 @@
       <c r="H24">
         <v>12</v>
       </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1523,6 +1541,9 @@
       <c r="H25">
         <v>8</v>
       </c>
+      <c r="I25">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1625,6 +1646,9 @@
       <c r="H30">
         <v>6</v>
       </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -1648,6 +1672,9 @@
       <c r="H31">
         <v>4</v>
       </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1672,7 +1699,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1694,8 +1721,11 @@
       <c r="H33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1717,8 +1747,11 @@
       <c r="H34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1738,7 +1771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1763,8 +1796,11 @@
       <c r="H36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1786,8 +1822,11 @@
       <c r="H37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1809,8 +1848,11 @@
       <c r="H38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1832,8 +1874,11 @@
       <c r="H39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1855,8 +1900,11 @@
       <c r="H40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1878,8 +1926,11 @@
       <c r="H41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1904,8 +1955,11 @@
       <c r="H42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1927,8 +1981,11 @@
       <c r="H43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1953,8 +2010,11 @@
       <c r="H44">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1977,6 +2037,10 @@
       <c r="H46">
         <f>SUM(H5:H44)</f>
         <v>79</v>
+      </c>
+      <c r="I46">
+        <f>SUM(I5:I44)</f>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>